<commit_message>
use "PERSON" designation instead of "NAME" for form-field type
</commit_message>
<xml_diff>
--- a/app/data-forms.xlsx
+++ b/app/data-forms.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">Person Providing Assistance</t>
   </si>
   <si>
-    <t xml:space="preserve">NAME</t>
+    <t xml:space="preserve">PERSON</t>
   </si>
   <si>
     <t xml:space="preserve">Dates of Assistance</t>
@@ -166,6 +166,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -250,16 +251,16 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.4744897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="63.4438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
include a uuid field in form spreadsheet and processing
</commit_message>
<xml_diff>
--- a/app/data-forms.xlsx
+++ b/app/data-forms.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t xml:space="preserve">Training</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Training-General</t>
   </si>
   <si>
+    <t xml:space="preserve">d6493bb0-a610-11e6-a350-8d1f5c467d3b</t>
+  </si>
+  <si>
     <t xml:space="preserve">Topic of Training</t>
   </si>
   <si>
@@ -55,6 +58,9 @@
     <t xml:space="preserve">Training-Institution</t>
   </si>
   <si>
+    <t xml:space="preserve">d6493bb1-a610-11e6-a350-8d1f5c467d3b</t>
+  </si>
+  <si>
     <t xml:space="preserve">Name of Institution</t>
   </si>
   <si>
@@ -73,6 +79,9 @@
     <t xml:space="preserve">Assistance-General</t>
   </si>
   <si>
+    <t xml:space="preserve">d6493bb2-a610-11e6-a350-8d1f5c467d3b</t>
+  </si>
+  <si>
     <t xml:space="preserve">Topic of Assistance</t>
   </si>
   <si>
@@ -94,6 +103,9 @@
     <t xml:space="preserve">Law, Regulation, and Policy-General</t>
   </si>
   <si>
+    <t xml:space="preserve">d6493bb3-a610-11e6-a350-8d1f5c467d3b</t>
+  </si>
+  <si>
     <t xml:space="preserve">Type</t>
   </si>
   <si>
@@ -118,6 +130,9 @@
     <t xml:space="preserve">Meeting-Basic</t>
   </si>
   <si>
+    <t xml:space="preserve">d6493bb4-a610-11e6-a350-8d1f5c467d3b</t>
+  </si>
+  <si>
     <t xml:space="preserve">Topic of Meeting</t>
   </si>
   <si>
@@ -133,12 +148,21 @@
     <t xml:space="preserve">Jurisdiction-Basic</t>
   </si>
   <si>
+    <t xml:space="preserve">d6493bb5-a610-11e6-a350-8d1f5c467d3b</t>
+  </si>
+  <si>
     <t xml:space="preserve">Name of Jurisdiction</t>
   </si>
   <si>
+    <t xml:space="preserve">JURISDICTION</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jurisdiction-Agency</t>
   </si>
   <si>
+    <t xml:space="preserve">d6493bb6-a610-11e6-a350-8d1f5c467d3b</t>
+  </si>
+  <si>
     <t xml:space="preserve">Name of Jurisdictional Agency</t>
   </si>
   <si>
@@ -146,6 +170,9 @@
   </si>
   <si>
     <t xml:space="preserve">Jurisdiction-Forest Monitoring Datasets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d6493bb7-a610-11e6-a350-8d1f5c467d3b</t>
   </si>
   <si>
     <t xml:space="preserve">Type of Data</t>
@@ -248,19 +275,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="63.4438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64.0918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.1530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="54.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -272,227 +301,248 @@
       <c r="B2" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
-        <v>38</v>
+      <c r="C30" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>3</v>
+      <c r="B31" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -500,31 +550,50 @@
         <v>40</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
-        <v>41</v>
+      <c r="C34" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="0" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="0" t="s">
+      <c r="B36" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="0" t="s">
         <v>43</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fully functional "JURISDICTION" form-field type
</commit_message>
<xml_diff>
--- a/app/data-forms.xlsx
+++ b/app/data-forms.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
   <si>
     <t xml:space="preserve">Training</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t xml:space="preserve">d6493bb5-a610-11e6-a350-8d1f5c467d3b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of Jurisdiction</t>
   </si>
   <si>
     <t xml:space="preserve">JURISDICTION</t>
@@ -275,21 +272,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.1530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="54.3214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="63.4438775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="53.5918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -515,31 +512,31 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="0" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="0" t="s">
+      <c r="B30" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>46</v>
+      <c r="D31" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>4</v>
@@ -547,53 +544,37 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>4</v>
+      <c r="B34" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="0" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" s="0" t="s">
+      <c r="C36" s="0" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="0" t="s">
+      <c r="D36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
include an INTEGER field type
</commit_message>
<xml_diff>
--- a/app/data-forms.xlsx
+++ b/app/data-forms.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Hours of Training</t>
   </si>
   <si>
-    <t xml:space="preserve">NUMBER</t>
+    <t xml:space="preserve">INTEGER</t>
   </si>
   <si>
     <t xml:space="preserve">Number of Men Attending</t>
@@ -275,18 +275,18 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="63.4438775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="53.5918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.6377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="52.9183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>